<commit_message>
Add collections data parsing and visualization to app
</commit_message>
<xml_diff>
--- a/data/map_data.xlsx
+++ b/data/map_data.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25915"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="-20" windowWidth="25600" windowHeight="17540" tabRatio="500"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Location</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>Annex</t>
+  </si>
+  <si>
+    <t>Harvard</t>
   </si>
 </sst>
 </file>
@@ -64,7 +67,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="136"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -431,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -536,6 +538,17 @@
       </c>
       <c r="C9">
         <v>0.115</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10">
+        <v>0.8</v>
+      </c>
+      <c r="C10">
+        <v>0.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>